<commit_message>
change `ieee-7012:7012Endpoint` to `Endpoint` #413
Co-authored-by: Arthit Suriyawongkul <arthit@gmail.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/ieee-7012.xlsx
+++ b/code/vocab_csv/ieee-7012.xlsx
@@ -359,10 +359,7 @@
     <t>A request to initiate negotiation with the goal of finding an acceptable agreement</t>
   </si>
   <si>
-    <t>7012Endpoint</t>
-  </si>
-  <si>
-    <t>7012 Endpoint</t>
+    <t>Endpoint</t>
   </si>
   <si>
     <t>A location that acts as an endpoint, such as a URL, for carrying out communications and interactions between parties as defined in IEEE 7012</t>
@@ -371,6 +368,9 @@
     <t>dpv:Location</t>
   </si>
   <si>
+    <t>modified</t>
+  </si>
+  <si>
     <t>AgreementInteractionRecord</t>
   </si>
   <si>
@@ -464,16 +464,16 @@
     <t>ieee-7012:PrivacyNegotiationRequest</t>
   </si>
   <si>
-    <t>has7012Endpoint</t>
-  </si>
-  <si>
-    <t>has 7012 endpoint</t>
+    <t>hasEndpoint</t>
+  </si>
+  <si>
+    <t>has endpoint</t>
   </si>
   <si>
     <t>Indicates the endpoint, such as a URL or an address, where 7012 related communications and interactions can be made</t>
   </si>
   <si>
-    <t>ieee-7012:7012Endpoint</t>
+    <t>ieee-7012:Endpoint</t>
   </si>
   <si>
     <t>hasHumanReadableFormat</t>
@@ -12535,13 +12535,13 @@
         <v>112</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="D7" s="14" t="s">
         <v>114</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>115</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>18</v>
@@ -12549,8 +12549,11 @@
       <c r="K7" s="8">
         <v>45643.0</v>
       </c>
+      <c r="L7" s="23">
+        <v>46056.0</v>
+      </c>
       <c r="M7" s="14" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8">
@@ -14892,9 +14895,11 @@
       <c r="K7" s="8">
         <v>45643.0</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="L7" s="8">
+        <v>46056.0</v>
+      </c>
       <c r="M7" s="5" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8">

</xml_diff>